<commit_message>
Planification et Documentation updated
</commit_message>
<xml_diff>
--- a/Documentation/Planification_TPI.xlsx
+++ b/Documentation/Planification_TPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\TipAlgoTri\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lelouch\Documents\TIPalgoTri\TipAlgoTri\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD65730-A30E-412E-9143-8ACCAE20E111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF33812-1087-4068-81C1-0BA24C9C5642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,39 +174,9 @@
     <t>Immersion (Création git, vérifications du poste, temps pour adapt.)</t>
   </si>
   <si>
-    <t>Faire le visuel du trie par insertion</t>
-  </si>
-  <si>
-    <t>Faire le visuel du trie à bulle</t>
-  </si>
-  <si>
-    <t>Faire le visuel du trieselection</t>
-  </si>
-  <si>
-    <t>Faire le visuel du trie à peigne</t>
-  </si>
-  <si>
-    <t>Faire le visuel du trie Shell</t>
-  </si>
-  <si>
     <t>Faire le visuel du form principal</t>
   </si>
   <si>
-    <t>Reglage de la vitesse d'éxécution du trie a bulle</t>
-  </si>
-  <si>
-    <t>Reglage de la vitesse d'éxécution du trie a peigne</t>
-  </si>
-  <si>
-    <t>Reglage de la vitesse d'éxécution du trie a séléction</t>
-  </si>
-  <si>
-    <t>Reglage de la vitesse d'éxécution du trie a insertion</t>
-  </si>
-  <si>
-    <t>Reglage de la vitesse d'éxécution du trie a shell</t>
-  </si>
-  <si>
     <t>Représenter de manière graphique /couleur différente. Bulle</t>
   </si>
   <si>
@@ -237,21 +207,6 @@
     <t>La hauteur représente son poids pour le tri à insertion</t>
   </si>
   <si>
-    <t>On peu mettre stop durant le tri à bulle</t>
-  </si>
-  <si>
-    <t>On peu mettre stop durant le tri à shell</t>
-  </si>
-  <si>
-    <t>On peu mettre stop durant le tri à peigne</t>
-  </si>
-  <si>
-    <t>On peu mettre stop durant le tri à selection</t>
-  </si>
-  <si>
-    <t>On peu mettre stop durant le tri à insertion</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ligne de code C# associée ou pseudo-code selon le choix en direct pour le tri à bulle.</t>
   </si>
   <si>
@@ -265,6 +220,51 @@
   </si>
   <si>
     <t xml:space="preserve"> ligne de code C# associée ou pseudo-code selon le choix en direct pour le tri à selection.</t>
+  </si>
+  <si>
+    <t>On peut mettre stop durant le tri à bulle</t>
+  </si>
+  <si>
+    <t>On peut mettre stop durant le tri à shell</t>
+  </si>
+  <si>
+    <t>On peut mettre stop durant le tri à peigne</t>
+  </si>
+  <si>
+    <t>On peut mettre stop durant le tri à selection</t>
+  </si>
+  <si>
+    <t>On peut mettre stop durant le tri à insertion</t>
+  </si>
+  <si>
+    <t>Réglage de la vitesse d'éxécution du tri à bulle</t>
+  </si>
+  <si>
+    <t>Réglage de la vitesse d'éxécution du tri à peigne</t>
+  </si>
+  <si>
+    <t>Réglage de la vitesse d'éxécution du tri à insertion</t>
+  </si>
+  <si>
+    <t>Réglage de la vitesse d'éxécution du tri à séléction</t>
+  </si>
+  <si>
+    <t>Réglage de la vitesse d'éxécution du tri Shell</t>
+  </si>
+  <si>
+    <t>Faire le visuel du tri Shell</t>
+  </si>
+  <si>
+    <t>Faire le visuel du tri à peigne</t>
+  </si>
+  <si>
+    <t>Faire le visuel du tri sélection</t>
+  </si>
+  <si>
+    <t>Faire le visuel du tri à bulle</t>
+  </si>
+  <si>
+    <t>Faire le visuel du tri par insertion</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="27"/>
       <c r="C2" s="6"/>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B4" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1182,13 +1182,13 @@
       <c r="K4" s="3"/>
       <c r="L4" s="11"/>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M28" si="0">SUM(C4:L4)</f>
+        <f t="shared" ref="M4:M18" si="0">SUM(C4:L4)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B5" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B6" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B7" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="B8" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" s="29">
         <v>4.1666666666666664E-2</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B12" s="29">
         <v>0.33333333333333331</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B13" s="29">
         <v>0.33333333333333331</v>
@@ -1359,13 +1359,13 @@
       <c r="J13" s="2"/>
       <c r="L13" s="11"/>
       <c r="M13" s="2">
-        <f t="shared" ref="M13:M17" si="1">SUM(C13:L13)</f>
+        <f t="shared" ref="M13:M16" si="1">SUM(C13:L13)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B14" s="29">
         <v>0.33333333333333331</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B15" s="29">
         <v>0.33333333333333331</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B16" s="29">
         <v>0.33333333333333331</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B18" s="29">
         <v>0.33333333333333331</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B19" s="29">
         <v>0.33333333333333331</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B20" s="29">
         <v>0.33333333333333331</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B21" s="29">
         <v>0.33333333333333331</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B22" s="29">
         <v>0.33333333333333331</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B24" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B25" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B26" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B27" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B28" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B30" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B31" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B32" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B33" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B34" s="29">
         <v>8.3333333333333329E-2</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B36" s="29">
         <v>1</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B37" s="29">
         <v>1</v>
@@ -1863,13 +1863,13 @@
       <c r="K37" s="3"/>
       <c r="L37" s="11"/>
       <c r="M37" s="2">
-        <f t="shared" ref="M37:M67" si="4">SUM(C37:L37)</f>
+        <f t="shared" ref="M37:M40" si="4">SUM(C37:L37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B38" s="29">
         <v>1</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B39" s="29">
         <v>1</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B40" s="29">
         <v>1</v>
@@ -2148,47 +2148,47 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
-        <f>SUM(B2:B51)</f>
+        <f t="shared" ref="B52:L52" si="5">SUM(B2:B51)</f>
         <v>11.124999999999998</v>
       </c>
       <c r="C52" s="2">
-        <f>SUM(C2:C51)</f>
+        <f t="shared" si="5"/>
         <v>1.125</v>
       </c>
       <c r="D52" s="2">
-        <f>SUM(D2:D51)</f>
+        <f t="shared" si="5"/>
         <v>0.14583333333333331</v>
       </c>
       <c r="E52" s="2">
-        <f>SUM(E2:E51)</f>
+        <f t="shared" si="5"/>
         <v>0.95833333333333337</v>
       </c>
       <c r="F52" s="2">
-        <f>SUM(F2:F51)</f>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G52" s="2">
-        <f>SUM(G2:G51)</f>
+        <f t="shared" si="5"/>
         <v>0.87499999999999978</v>
       </c>
       <c r="H52" s="2">
-        <f>SUM(H2:H51)</f>
+        <f t="shared" si="5"/>
         <v>0.20833333333333331</v>
       </c>
       <c r="I52" s="2">
-        <f>SUM(I2:I51)</f>
+        <f t="shared" si="5"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="J52" s="2">
-        <f>SUM(J2:J51)</f>
+        <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K52" s="2">
-        <f>SUM(K2:K51)</f>
+        <f t="shared" si="5"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="L52" s="2">
-        <f>SUM(L2:L51)</f>
+        <f t="shared" si="5"/>
         <v>0.20833333333333334</v>
       </c>
     </row>

</xml_diff>